<commit_message>
fix : "RPA Calendar v2 데이터 DB에 저장"
파일 다운로드 및 업로드 방식에서, day 0으로 하여 기본 입력값을 저장할 행을 넣는 것으로 가정하여 calender의 html 코드 저장 및 불러오기로 html에 삽입.
</commit_message>
<xml_diff>
--- a/src/main/resources/uipath/result/test2.xlsx
+++ b/src/main/resources/uipath/result/test2.xlsx
@@ -24,53 +24,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>3
-학생 독립운동 기념일</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>31
+세계 금연의 날
+바다의 날</t>
   </si>
   <si>
     <t>4
-점자의 날</t>
-  </si>
-  <si>
-    <t>5
-소상공인의 날</t>
-  </si>
-  <si>
-    <t>8
-입동</t>
-  </si>
-  <si>
-    <t>9
-소방의 날</t>
-  </si>
-  <si>
-    <t>11
-유엔참전용사 국제추모식
-보행자의 날
-농업인의 날</t>
-  </si>
-  <si>
-    <t>13
-음10.1</t>
-  </si>
-  <si>
-    <t>17
-순국선열의 날</t>
-  </si>
-  <si>
-    <t>19
-아동학대예방의날</t>
-  </si>
-  <si>
-    <t>22
-소설
-김치의 날</t>
-  </si>
-  <si>
-    <t>27
-음10.15</t>
+지식재산의 날</t>
+  </si>
+  <si>
+    <t>7
+음8.1
+백로
+푸른하늘의날</t>
+  </si>
+  <si>
+    <t>10
+세계 자살예방의 날
+9.10 해양경찰의날</t>
+  </si>
+  <si>
+    <t>18
+청년의날</t>
+  </si>
+  <si>
+    <t>21
+음8.15
+추석
+치매극복의 날</t>
+  </si>
+  <si>
+    <t>23
+추분</t>
   </si>
 </sst>
 </file>
@@ -398,58 +385,58 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="72.5">
-      <c r="A1">
+    <row r="1" spans="1:7" ht="43.5">
+      <c r="A1" s="1">
         <v>29</v>
       </c>
       <c r="B1" s="1">
         <v>30</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="1">
         <v>31</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>1</v>
       </c>
       <c r="E1" s="1">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
+      <c r="F1" s="1">
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="130.5">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
+    <row r="2" spans="1:7" ht="101.5">
+      <c r="A2" s="1">
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
+      <c r="G2" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.5">
       <c r="A3" s="1">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+      <c r="B3" s="1">
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>14</v>
@@ -460,28 +447,28 @@
       <c r="E3" s="1">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1">
-        <v>18</v>
+      <c r="F3" s="1">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="58">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
+    <row r="4" spans="1:7" ht="72.5">
+      <c r="A4" s="1">
+        <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>20</v>
       </c>
-      <c r="C4" s="1">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1">
-        <v>23</v>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="F4" s="1">
         <v>24</v>
@@ -490,12 +477,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29">
-      <c r="A5">
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
         <v>26</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
+      <c r="B5" s="1">
+        <v>27</v>
       </c>
       <c r="C5" s="1">
         <v>28</v>
@@ -503,37 +490,37 @@
       <c r="D5" s="1">
         <v>29</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>30</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="87">
       <c r="A6">
         <v>30</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>3</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>4</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>5</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix : "RPA Calendar v2 수정"
마지막 수정으로, RPA 적용에 관련된 내용 대폭 변경 예정.
</commit_message>
<xml_diff>
--- a/src/main/resources/uipath/result/test2.xlsx
+++ b/src/main/resources/uipath/result/test2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="10100"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19180" windowHeight="10100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,40 +24,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>31
 세계 금연의 날
 바다의 날</t>
   </si>
   <si>
-    <t>4
-지식재산의 날</t>
-  </si>
-  <si>
-    <t>7
-음8.1
-백로
-푸른하늘의날</t>
+    <t>1
+의병의 날</t>
+  </si>
+  <si>
+    <t>3
+음4.15</t>
+  </si>
+  <si>
+    <t>5
+환경의 날</t>
+  </si>
+  <si>
+    <t>6
+현충일
+망종</t>
   </si>
   <si>
     <t>10
-세계 자살예방의 날
-9.10 해양경찰의날</t>
+6.10 민주항쟁기념일</t>
+  </si>
+  <si>
+    <t>15
+노인학대 예방의 날</t>
   </si>
   <si>
     <t>18
-청년의날</t>
+음5.1</t>
   </si>
   <si>
     <t>21
-음8.15
-추석
-치매극복의 날</t>
-  </si>
-  <si>
-    <t>23
-추분</t>
+하지
+해양조사의 날</t>
+  </si>
+  <si>
+    <t>22
+단오</t>
+  </si>
+  <si>
+    <t>25
+6·25 전쟁일</t>
+  </si>
+  <si>
+    <t>28
+철도의 날</t>
   </si>
 </sst>
 </file>
@@ -387,117 +404,117 @@
   <sheetData>
     <row r="1" spans="1:7" ht="43.5">
       <c r="A1" s="1">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1">
         <v>29</v>
       </c>
-      <c r="B1" s="1">
+      <c r="C1" s="1">
         <v>30</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>31</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>2</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="72.5">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="72.5">
+      <c r="A3" s="1">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="58">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.5">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="101.5">
-      <c r="A2" s="1">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.5">
-      <c r="A3" s="1">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1">
-        <v>17</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="72.5">
-      <c r="A4" s="1">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>22</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1">
-        <v>24</v>
-      </c>
-      <c r="G4" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1">
-        <v>30</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="87">

</xml_diff>